<commit_message>
Small edits to prepare the repository for first submission
- Complete ReadMe
- SEM plots without acronymes
- Current version of MS as MS-Doc
</commit_message>
<xml_diff>
--- a/div/setting_generic_model.xlsx
+++ b/div/setting_generic_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobias/Documents/Dropbox/Schreibtisch_Ro/1568_Publi-NDep-Tagfalter/10-GitHub-NDep_butterflies/div/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8339167D-1E00-EA4A-A15B-CB8B02996343}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F272EDE6-FC3A-B645-B488-EA89DA9F62D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28820" windowHeight="17540" xr2:uid="{CA667B0F-BF01-B64F-B24B-AAA21C91837C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{CA667B0F-BF01-B64F-B24B-AAA21C91837C}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes_generic" sheetId="1" r:id="rId1"/>
@@ -168,12 +168,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>Butterfly species\nrichness (BSR)</t>
-  </si>
-  <si>
-    <t>Plant species\nrichness (PSR)</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -184,6 +178,12 @@
   </si>
   <si>
     <t>Nitrogen\ndeposition</t>
+  </si>
+  <si>
+    <t>Butterfly species\nrichness</t>
+  </si>
+  <si>
+    <t>Plant species\nrichness</t>
   </si>
 </sst>
 </file>
@@ -592,9 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0D789B-A875-9D45-B30C-CB93EB950AEC}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -737,7 +735,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1109,9 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BA3A3FC-8C43-274B-A8FC-6B6E1A779833}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1159,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D2">
         <v>0.75</v>
@@ -1191,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D3">
         <v>1.75</v>
@@ -1284,10 +1280,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
         <v>49</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
       </c>
       <c r="D6">
         <v>2.25</v>
@@ -1348,7 +1344,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>42</v>
@@ -1545,10 +1541,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <f>$D$7 + 0.3</f>

</xml_diff>